<commit_message>
Make xls for selected stations, final maps
</commit_message>
<xml_diff>
--- a/01_Station_positions_for_map.xlsx
+++ b/01_Station_positions_for_map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Hjelp\Maps-Oslofjord\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80F8DBE-30F7-4197-8E50-6B23415B9000}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC7CD78-F0C2-49FF-8C9E-FD1189AE6C92}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="2085" windowWidth="23115" windowHeight="14295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="191">
   <si>
     <t>Project</t>
   </si>
@@ -946,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1842,6 +1842,9 @@
       </c>
       <c r="C26" t="s">
         <v>122</v>
+      </c>
+      <c r="D26" t="s">
+        <v>186</v>
       </c>
       <c r="E26">
         <v>9.6180000000000003</v>

</xml_diff>